<commit_message>
scan folder win add
</commit_message>
<xml_diff>
--- a/folder_scan.xlsx
+++ b/folder_scan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>no</t>
   </si>
@@ -29,6 +29,54 @@
   </si>
   <si>
     <t>f_link</t>
+  </si>
+  <si>
+    <t>C:/TEMP</t>
+  </si>
+  <si>
+    <t>C:/TEMP\TCO_20160823</t>
+  </si>
+  <si>
+    <t>controldebug.ini</t>
+  </si>
+  <si>
+    <t>friend_list.txt</t>
+  </si>
+  <si>
+    <t>SharedDisable.exe</t>
+  </si>
+  <si>
+    <t>stop.lnk</t>
+  </si>
+  <si>
+    <t>wushowhide.diagcab</t>
+  </si>
+  <si>
+    <t>data1.cab</t>
+  </si>
+  <si>
+    <t>data1.hdr</t>
+  </si>
+  <si>
+    <t>data2.cab</t>
+  </si>
+  <si>
+    <t>ikernel.ex_</t>
+  </si>
+  <si>
+    <t>layout.bin</t>
+  </si>
+  <si>
+    <t>Setup.exe</t>
+  </si>
+  <si>
+    <t>Setup.ini</t>
+  </si>
+  <si>
+    <t>setup.inx</t>
+  </si>
+  <si>
+    <t>SVRINFO.INI</t>
   </si>
 </sst>
 </file>
@@ -386,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,6 +457,272 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <f>HYPERLINK("C:/TEMP", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <f>HYPERLINK("C:/TEMP\controldebug.ini", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <f>HYPERLINK("C:/TEMP", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <f>HYPERLINK("C:/TEMP\friend_list.txt", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f>HYPERLINK("C:/TEMP", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <f>HYPERLINK("C:/TEMP\SharedDisable.exe", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f>HYPERLINK("C:/TEMP", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <f>HYPERLINK("C:/TEMP\stop.lnk", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>HYPERLINK("C:/TEMP", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <f>HYPERLINK("C:/TEMP\wushowhide.diagcab", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823\data1.cab", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823\data1.hdr", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823\data2.cab", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823\ikernel.ex_", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823\layout.bin", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823\Setup.exe", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823\Setup.ini", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823\setup.inx", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823", "DirView")</f>
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <f>HYPERLINK("C:/TEMP\TCO_20160823\SVRINFO.INI", "FileView")</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>